<commit_message>
Fixed bugs on students and timetables
</commit_message>
<xml_diff>
--- a/examples/example_timetable.xlsx
+++ b/examples/example_timetable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giulia/Desktop/Polito/Da dare/Software Engineering II/Project/se2-groupD/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{27D5E8D1-BD67-914F-9666-EC39B448E130}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3C060B81-4880-EB43-A650-D883F2FC97B8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16180" xr2:uid="{75790267-ED11-6C4B-A070-A538B8C5B55B}"/>
   </bookViews>
@@ -439,7 +439,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fixed bugs on students and timetables (#111)
</commit_message>
<xml_diff>
--- a/examples/example_timetable.xlsx
+++ b/examples/example_timetable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giulia/Desktop/Polito/Da dare/Software Engineering II/Project/se2-groupD/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{27D5E8D1-BD67-914F-9666-EC39B448E130}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3C060B81-4880-EB43-A650-D883F2FC97B8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16180" xr2:uid="{75790267-ED11-6C4B-A070-A538B8C5B55B}"/>
   </bookViews>
@@ -439,7 +439,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>